<commit_message>
Aggregation des cartes verticalement, correction de typos
</commit_message>
<xml_diff>
--- a/src/resources/deplacements.xlsx
+++ b/src/resources/deplacements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsaban/git/perso/ficanasse-cardgame/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13CCEFE-97FD-814F-AD28-75FD7E9455DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B94803-71F5-494A-8FDD-CE78BAE2B578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7593484B-EC08-A64B-98EC-E341B0114FA2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{7593484B-EC08-A64B-98EC-E341B0114FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,8 +118,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A67FF59-AF14-5249-9575-C8E32E6F0A0E}" name="Table1" displayName="Table1" ref="A1:F61" totalsRowShown="0">
-  <autoFilter ref="A1:F61" xr:uid="{AFF52647-ECCC-524C-BAA0-21786BA5E8BF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A67FF59-AF14-5249-9575-C8E32E6F0A0E}" name="Table1" displayName="Table1" ref="A1:F64" totalsRowShown="0">
+  <autoFilter ref="A1:F64" xr:uid="{AFF52647-ECCC-524C-BAA0-21786BA5E8BF}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{341AA4DC-D473-AB4D-9EEA-D930F78A8F20}" name="id"/>
     <tableColumn id="2" xr3:uid="{769CA09F-2520-4547-A028-04700D833DDC}" name="Lieu1" dataDxfId="0">
@@ -438,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE4C0BA-4279-594D-A79C-14FA55DC4F39}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,23 +483,23 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:F33" ca="1" si="0">VLOOKUP(ROUND(RAND()*COUNT($J$1:$J$32)+1, 0),$I$1:$J$32,2,TRUE)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -513,23 +514,23 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -544,23 +545,23 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I4">
         <v>4</v>
@@ -575,15 +576,15 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
@@ -591,7 +592,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I5">
         <v>5</v>
@@ -606,19 +607,19 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
@@ -637,11 +638,11 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
@@ -649,11 +650,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I7">
         <v>7</v>
@@ -668,11 +669,11 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
@@ -680,11 +681,11 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I8">
         <v>8</v>
@@ -699,7 +700,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
@@ -707,7 +708,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
@@ -730,23 +731,23 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I10">
         <v>10</v>
@@ -761,23 +762,23 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I11">
         <v>11</v>
@@ -796,7 +797,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
@@ -804,11 +805,11 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I12">
         <v>12</v>
@@ -823,19 +824,19 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
@@ -854,23 +855,23 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I14">
         <v>14</v>
@@ -889,11 +890,11 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
@@ -901,7 +902,7 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15">
         <v>15</v>
@@ -920,7 +921,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
@@ -928,11 +929,11 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I16">
         <v>16</v>
@@ -955,7 +956,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
@@ -963,7 +964,7 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I17">
         <v>17</v>
@@ -978,19 +979,19 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
@@ -1009,23 +1010,23 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I19">
         <v>19</v>
@@ -1040,23 +1041,23 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I20">
         <v>20</v>
@@ -1071,23 +1072,23 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I21">
         <v>21</v>
@@ -1102,7 +1103,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
@@ -1110,15 +1111,15 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I22">
         <v>22</v>
@@ -1133,11 +1134,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
@@ -1145,11 +1146,11 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I23">
         <v>23</v>
@@ -1164,23 +1165,23 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="E24">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
       <c r="F24">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I24">
         <v>24</v>
@@ -1195,23 +1196,23 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I25">
         <v>25</v>
@@ -1230,19 +1231,19 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I26">
         <v>26</v>
@@ -1257,23 +1258,23 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I27">
         <v>27</v>
@@ -1288,23 +1289,23 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I28">
         <v>28</v>
@@ -1319,15 +1320,15 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
@@ -1335,7 +1336,7 @@
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I29">
         <v>29</v>
@@ -1350,23 +1351,23 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I30">
         <v>30</v>
@@ -1385,19 +1386,19 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I31">
         <v>31</v>
@@ -1412,7 +1413,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
@@ -1420,15 +1421,15 @@
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I32">
         <v>32</v>
@@ -1443,23 +1444,23 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1468,11 +1469,11 @@
       </c>
       <c r="B34">
         <f t="shared" ref="B34:F61" ca="1" si="1">VLOOKUP(ROUND(RAND()*COUNT($J$1:$J$32)+1, 0),$I$1:$J$32,2,TRUE)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
@@ -1480,11 +1481,11 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1493,23 +1494,23 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1522,19 +1523,19 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1543,15 +1544,15 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="1"/>
@@ -1568,23 +1569,23 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1593,7 +1594,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="1"/>
@@ -1601,11 +1602,11 @@
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="1"/>
@@ -1618,11 +1619,11 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="1"/>
@@ -1630,7 +1631,7 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="1"/>
@@ -1643,23 +1644,23 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
-      <c r="C41">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
       <c r="D41">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1668,7 +1669,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="1"/>
@@ -1676,15 +1677,15 @@
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1693,19 +1694,19 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="1"/>
@@ -1718,23 +1719,23 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1747,7 +1748,7 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="1"/>
@@ -1759,7 +1760,7 @@
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1768,19 +1769,19 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="1"/>
@@ -1797,19 +1798,19 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1818,23 +1819,23 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1843,11 +1844,11 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="1"/>
@@ -1859,7 +1860,7 @@
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1868,23 +1869,23 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1893,23 +1894,23 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1918,23 +1919,23 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1943,23 +1944,23 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1968,11 +1969,11 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="1"/>
@@ -1980,11 +1981,11 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1993,23 +1994,23 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2018,23 +2019,23 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2051,11 +2052,11 @@
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="1"/>
@@ -2068,23 +2069,23 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2093,7 +2094,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="1"/>
@@ -2101,15 +2102,15 @@
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2118,11 +2119,11 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="1"/>
@@ -2130,11 +2131,11 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2143,23 +2144,98 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="1"/>
         <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <f t="shared" ref="B62:B64" ca="1" si="2">VLOOKUP(ROUND(RAND()*COUNT($J$1:$J$32)+1, 0),$I$1:$J$32,2,TRUE)</f>
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <f t="shared" ref="C62:C64" ca="1" si="3">VLOOKUP(ROUND(RAND()*COUNT($J$1:$J$32)+1, 0),$I$1:$J$32,2,TRUE)</f>
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ref="D62:D64" ca="1" si="4">VLOOKUP(ROUND(RAND()*COUNT($J$1:$J$32)+1, 0),$I$1:$J$32,2,TRUE)</f>
+        <v>9</v>
+      </c>
+      <c r="E62">
+        <f t="shared" ref="E62:E64" ca="1" si="5">VLOOKUP(ROUND(RAND()*COUNT($J$1:$J$32)+1, 0),$I$1:$J$32,2,TRUE)</f>
+        <v>7</v>
+      </c>
+      <c r="F62">
+        <f t="shared" ref="F62:F64" ca="1" si="6">VLOOKUP(ROUND(RAND()*COUNT($J$1:$J$32)+1, 0),$I$1:$J$32,2,TRUE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ca="1" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="E63">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="F63">
+        <f t="shared" ca="1" si="6"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="D64">
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="E64">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="F64">
+        <f t="shared" ca="1" si="6"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>